<commit_message>
Oppdateringer av kodelister og korrigering av pekere til eksempler på mva-melding.
</commit_message>
<xml_diff>
--- a/docs/documentation/forretningsregler/revidert-protoype-mvamelding.xlsx
+++ b/docs/documentation/forretningsregler/revidert-protoype-mvamelding.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://samhandling.skead.no/sites/MVAsatsning/Delte dokumenter/07 Forretningsutvikling/mva-melding/Utforming av mva-melding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k97594\Documents\prosjekter\mva-meldingen\docs\english\informasjonsmodell\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25248" windowHeight="10284"/>
   </bookViews>
   <sheets>
     <sheet name="Eksempel på mva-melding" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="133">
   <si>
     <t>Uttak</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Termin</t>
   </si>
   <si>
-    <t>Erstatter melding</t>
-  </si>
-  <si>
     <t>Melding nummer</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
     <t>zzx 4.34.3</t>
   </si>
   <si>
-    <t>2021-2</t>
-  </si>
-  <si>
     <t>MVAkode regnskap</t>
   </si>
   <si>
@@ -363,9 +357,6 @@
     <t>Omsetning 15%</t>
   </si>
   <si>
-    <t>Bankkonto</t>
-  </si>
-  <si>
     <t>KID</t>
   </si>
   <si>
@@ -387,9 +378,6 @@
     <t>Spesifikasjon</t>
   </si>
   <si>
-    <t>Denne er usikker</t>
-  </si>
-  <si>
     <t>Sats</t>
   </si>
   <si>
@@ -427,6 +415,15 @@
   </si>
   <si>
     <t>Grunnlag</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>År</t>
+  </si>
+  <si>
+    <t>mars-april</t>
   </si>
 </sst>
 </file>
@@ -682,13 +679,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -732,24 +729,6 @@
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Fortegn er som i bokføringen</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nb-NO"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -1157,62 +1136,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G38"/>
+  <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>93</v>
-      </c>
       <c r="C6" s="20"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1220,209 +1199,223 @@
         <v>913238254</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="11">
         <v>2396</v>
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>8</v>
+        <v>119</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="24"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="24"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23">
+        <f>SUM(F25:F33)</f>
+        <v>-11500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="str">
-        <f>"Sum "&amp;IF(F24&lt;0,"å betale",IF(F24=0,"","tilgode"))</f>
-        <v>Sum å betale</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23">
-        <f>SUM(F27:F35)</f>
-        <v>-11500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="3">
+        <v>-200000</v>
+      </c>
+      <c r="E25" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="F25" s="3">
+        <v>-50000</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="3">
+        <v>-100000</v>
+      </c>
+      <c r="E26" s="26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D27" s="3">
-        <v>-200000</v>
+        <v>-10000</v>
       </c>
       <c r="E27" s="26">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="F27" s="3">
-        <v>-50000</v>
+        <v>-1500</v>
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="3">
-        <v>-100000</v>
-      </c>
-      <c r="E28" s="26">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3">
+        <v>30000</v>
+      </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="3">
-        <v>-10000</v>
-      </c>
-      <c r="E29" s="26">
-        <v>0.15</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="3">
-        <v>-1500</v>
+        <v>10000</v>
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
-        <v>41</v>
-      </c>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
       <c r="B30" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>128</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="3">
-        <v>30000</v>
-      </c>
+      <c r="F30" s="3"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
-        <v>41</v>
-      </c>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="21"/>
       <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="3">
-        <v>10000</v>
-      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
@@ -1430,10 +1423,10 @@
       <c r="F32" s="3"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
       <c r="B33" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
@@ -1441,43 +1434,21 @@
       <c r="F33" s="3"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="10"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1490,19 +1461,19 @@
           <x14:formula1>
             <xm:f>Koder!$A$5:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B27:B35</xm:sqref>
+          <xm:sqref>B25:B33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Koder!$I$6:$I$39</xm:f>
           </x14:formula1>
-          <xm:sqref>A27:A35 C32:C34</xm:sqref>
+          <xm:sqref>A25:A33 C30:C32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Koder!$A$15:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1518,21 +1489,21 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L25" s="28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L26" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1556,966 +1527,966 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5546875" customWidth="1"/>
     <col min="5" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E9">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E10">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E11">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E12">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E13">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E14">
         <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E15">
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E17">
         <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O17" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17" t="s">
         <v>63</v>
       </c>
-      <c r="Q17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E19">
         <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E20">
         <v>5</v>
       </c>
       <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
-        <v>21</v>
-      </c>
       <c r="H20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E21">
         <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E22">
         <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E24">
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E25">
         <v>81</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E26">
         <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E27">
         <v>83</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E28">
         <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E29">
         <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E30">
         <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E31">
         <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E32">
         <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E33">
         <v>89</v>
       </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E34">
         <v>91</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>92</v>
       </c>
       <c r="F35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
         <v>32</v>
       </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>33</v>
-      </c>
       <c r="I35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
         <v>11</v>
       </c>
-      <c r="G36" t="s">
-        <v>12</v>
-      </c>
       <c r="H36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="5:15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E40">
         <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E41">
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="5:15" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E42">
         <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E43">
         <v>22</v>
       </c>
       <c r="F43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E44">
         <v>81</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E45">
         <v>82</v>
       </c>
       <c r="F45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E46">
         <v>83</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E47">
         <v>84</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E48">
         <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E49">
         <v>86</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H49" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E50">
         <v>87</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E51">
         <v>88</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H51" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E52">
         <v>89</v>
       </c>
       <c r="F52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E53">
         <v>91</v>
       </c>
       <c r="F53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E54">
         <v>92</v>
       </c>
       <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
         <v>32</v>
-      </c>
-      <c r="G54" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2532,14 +2503,14 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2547,9 +2518,9 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -2557,75 +2528,75 @@
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>91</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>93</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="20"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="2">
         <v>913238254</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2">
         <v>897455341</v>
@@ -2640,14 +2611,14 @@
         <v>-200000</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="3">
         <f>F15*0.25</f>
         <v>-50000</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2">
         <v>897455341</v>
@@ -2662,11 +2633,11 @@
         <v>-100000</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>971648652</v>
       </c>
@@ -2681,14 +2652,14 @@
         <v>120000</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" ref="H17" si="0">F17*0.25</f>
         <v>30000</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2697,10 +2668,10 @@
       <c r="G18" s="2"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E20" s="7"/>
     </row>
   </sheetData>
@@ -2722,17 +2693,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100771C32DEAFFE3B4B96D01FE0FE913B3B" ma:contentTypeVersion="20" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="aede315d5b925a07e5cacaa0ceea4b20">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8002682317f967cbab1e2c1a7ba68677" ns2:_="">
     <xsd:import namespace="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
@@ -2880,7 +2840,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B3C8295-E26A-42EC-B317-A8E3F84A435E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A608ABE4-968C-40FB-B935-536F1C772DAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2896,28 +2885,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38C39DB4-0F3C-4908-BCEE-BD79F50A7EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B3C8295-E26A-42EC-B317-A8E3F84A435E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Oppdateringer av kodelister og korrigering av pekere til eksempler på mva-melding. (#46)
</commit_message>
<xml_diff>
--- a/docs/documentation/forretningsregler/revidert-protoype-mvamelding.xlsx
+++ b/docs/documentation/forretningsregler/revidert-protoype-mvamelding.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://samhandling.skead.no/sites/MVAsatsning/Delte dokumenter/07 Forretningsutvikling/mva-melding/Utforming av mva-melding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k97594\Documents\prosjekter\mva-meldingen\docs\english\informasjonsmodell\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25248" windowHeight="10284"/>
   </bookViews>
   <sheets>
     <sheet name="Eksempel på mva-melding" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="133">
   <si>
     <t>Uttak</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Termin</t>
   </si>
   <si>
-    <t>Erstatter melding</t>
-  </si>
-  <si>
     <t>Melding nummer</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
     <t>zzx 4.34.3</t>
   </si>
   <si>
-    <t>2021-2</t>
-  </si>
-  <si>
     <t>MVAkode regnskap</t>
   </si>
   <si>
@@ -363,9 +357,6 @@
     <t>Omsetning 15%</t>
   </si>
   <si>
-    <t>Bankkonto</t>
-  </si>
-  <si>
     <t>KID</t>
   </si>
   <si>
@@ -387,9 +378,6 @@
     <t>Spesifikasjon</t>
   </si>
   <si>
-    <t>Denne er usikker</t>
-  </si>
-  <si>
     <t>Sats</t>
   </si>
   <si>
@@ -427,6 +415,15 @@
   </si>
   <si>
     <t>Grunnlag</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>År</t>
+  </si>
+  <si>
+    <t>mars-april</t>
   </si>
 </sst>
 </file>
@@ -682,13 +679,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -732,24 +729,6 @@
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Fortegn er som i bokføringen</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nb-NO"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -1157,62 +1136,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G38"/>
+  <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>93</v>
-      </c>
       <c r="C6" s="20"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1220,209 +1199,223 @@
         <v>913238254</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="11">
         <v>2396</v>
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>8</v>
+        <v>119</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="24"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="24"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23">
+        <f>SUM(F25:F33)</f>
+        <v>-11500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="str">
-        <f>"Sum "&amp;IF(F24&lt;0,"å betale",IF(F24=0,"","tilgode"))</f>
-        <v>Sum å betale</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23">
-        <f>SUM(F27:F35)</f>
-        <v>-11500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="3">
+        <v>-200000</v>
+      </c>
+      <c r="E25" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="F25" s="3">
+        <v>-50000</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="3">
+        <v>-100000</v>
+      </c>
+      <c r="E26" s="26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D27" s="3">
-        <v>-200000</v>
+        <v>-10000</v>
       </c>
       <c r="E27" s="26">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="F27" s="3">
-        <v>-50000</v>
+        <v>-1500</v>
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="3">
-        <v>-100000</v>
-      </c>
-      <c r="E28" s="26">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3">
+        <v>30000</v>
+      </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="3">
-        <v>-10000</v>
-      </c>
-      <c r="E29" s="26">
-        <v>0.15</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="3">
-        <v>-1500</v>
+        <v>10000</v>
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
-        <v>41</v>
-      </c>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
       <c r="B30" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>128</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="3">
-        <v>30000</v>
-      </c>
+      <c r="F30" s="3"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
-        <v>41</v>
-      </c>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="21"/>
       <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="3">
-        <v>10000</v>
-      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
@@ -1430,10 +1423,10 @@
       <c r="F32" s="3"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
       <c r="B33" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
@@ -1441,43 +1434,21 @@
       <c r="F33" s="3"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="10"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1490,19 +1461,19 @@
           <x14:formula1>
             <xm:f>Koder!$A$5:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B27:B35</xm:sqref>
+          <xm:sqref>B25:B33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Koder!$I$6:$I$39</xm:f>
           </x14:formula1>
-          <xm:sqref>A27:A35 C32:C34</xm:sqref>
+          <xm:sqref>A25:A33 C30:C32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Koder!$A$15:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1518,21 +1489,21 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L25" s="28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L26" s="27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1556,966 +1527,966 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5546875" customWidth="1"/>
     <col min="5" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E9">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E10">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E11">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E12">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E13">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E14">
         <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E15">
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E17">
         <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O17" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17" t="s">
         <v>63</v>
       </c>
-      <c r="Q17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E19">
         <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E20">
         <v>5</v>
       </c>
       <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
-        <v>21</v>
-      </c>
       <c r="H20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E21">
         <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E22">
         <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E24">
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E25">
         <v>81</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E26">
         <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E27">
         <v>83</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E28">
         <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E29">
         <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E30">
         <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E31">
         <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E32">
         <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E33">
         <v>89</v>
       </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E34">
         <v>91</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>92</v>
       </c>
       <c r="F35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
         <v>32</v>
       </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>33</v>
-      </c>
       <c r="I35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
         <v>11</v>
       </c>
-      <c r="G36" t="s">
-        <v>12</v>
-      </c>
       <c r="H36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="5:15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E40">
         <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E41">
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="5:15" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E42">
         <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E43">
         <v>22</v>
       </c>
       <c r="F43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E44">
         <v>81</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E45">
         <v>82</v>
       </c>
       <c r="F45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="5:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E46">
         <v>83</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E47">
         <v>84</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="5:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E48">
         <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E49">
         <v>86</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H49" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E50">
         <v>87</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E51">
         <v>88</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H51" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E52">
         <v>89</v>
       </c>
       <c r="F52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E53">
         <v>91</v>
       </c>
       <c r="F53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E54">
         <v>92</v>
       </c>
       <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
         <v>32</v>
-      </c>
-      <c r="G54" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2532,14 +2503,14 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2547,9 +2518,9 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -2557,75 +2528,75 @@
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>91</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>93</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="20"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="2">
         <v>913238254</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2">
         <v>897455341</v>
@@ -2640,14 +2611,14 @@
         <v>-200000</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="3">
         <f>F15*0.25</f>
         <v>-50000</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2">
         <v>897455341</v>
@@ -2662,11 +2633,11 @@
         <v>-100000</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>971648652</v>
       </c>
@@ -2681,14 +2652,14 @@
         <v>120000</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" ref="H17" si="0">F17*0.25</f>
         <v>30000</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2697,10 +2668,10 @@
       <c r="G18" s="2"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E20" s="7"/>
     </row>
   </sheetData>
@@ -2722,17 +2693,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100771C32DEAFFE3B4B96D01FE0FE913B3B" ma:contentTypeVersion="20" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="aede315d5b925a07e5cacaa0ceea4b20">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8002682317f967cbab1e2c1a7ba68677" ns2:_="">
     <xsd:import namespace="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
@@ -2880,7 +2840,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B3C8295-E26A-42EC-B317-A8E3F84A435E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A608ABE4-968C-40FB-B935-536F1C772DAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2896,28 +2885,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38C39DB4-0F3C-4908-BCEE-BD79F50A7EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B3C8295-E26A-42EC-B317-A8E3F84A435E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>